<commit_message>
Assembled markdown table of data dictionary
</commit_message>
<xml_diff>
--- a/data-documentation/data-documentation.xlsx
+++ b/data-documentation/data-documentation.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lanel\OneDrive\Documents\R\k-entry\data-documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="175" documentId="113_{3FDA6900-4998-4D14-B81F-B921EDAF6AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5DAB02C8-A6D0-43BB-AD00-45E3D55D18D1}"/>
+  <xr:revisionPtr revIDLastSave="177" documentId="113_{3FDA6900-4998-4D14-B81F-B921EDAF6AC8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{40266C78-11AD-42D1-851F-D802A52B04BF}"/>
   <bookViews>
-    <workbookView xWindow="1455" yWindow="1230" windowWidth="11130" windowHeight="9480" firstSheet="1" activeTab="1" xr2:uid="{32B1247A-B1EE-4DD4-8B74-E50A379266F9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{32B1247A-B1EE-4DD4-8B74-E50A379266F9}"/>
   </bookViews>
   <sheets>
     <sheet name="Census Workflow" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="650">
   <si>
     <t>Variable name</t>
   </si>
@@ -2228,15 +2228,15 @@
     <xf numFmtId="0" fontId="8" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -4155,7 +4155,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G134" sqref="G134"/>
+      <selection pane="bottomLeft" activeCell="E129" sqref="E129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5303,7 +5303,7 @@
       <c r="I52" s="7"/>
       <c r="J52" s="1"/>
     </row>
-    <row r="53" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:10" ht="75" x14ac:dyDescent="0.25">
       <c r="C53" s="1" t="s">
         <v>65</v>
       </c>
@@ -5699,7 +5699,7 @@
       <c r="C72" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="D72" s="26" t="s">
+      <c r="D72" s="25" t="s">
         <v>590</v>
       </c>
       <c r="E72" s="1" t="s">
@@ -6866,7 +6866,7 @@
       <c r="C130" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="D130" s="27" t="s">
+      <c r="D130" s="26" t="s">
         <v>597</v>
       </c>
       <c r="E130" s="1" t="s">
@@ -6886,7 +6886,7 @@
       <c r="C131" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="D131" s="27" t="s">
+      <c r="D131" s="26" t="s">
         <v>596</v>
       </c>
       <c r="E131" s="1" t="s">
@@ -6929,7 +6929,9 @@
       <c r="D133" s="1" t="s">
         <v>630</v>
       </c>
-      <c r="E133" s="1"/>
+      <c r="E133" s="1" t="s">
+        <v>600</v>
+      </c>
       <c r="F133" s="1" t="s">
         <v>606</v>
       </c>
@@ -6945,7 +6947,9 @@
       <c r="D134" s="1" t="s">
         <v>631</v>
       </c>
-      <c r="E134" s="1"/>
+      <c r="E134" s="1" t="s">
+        <v>600</v>
+      </c>
       <c r="F134" s="1" t="s">
         <v>606</v>
       </c>
@@ -6958,7 +6962,7 @@
       <c r="C135" s="1" t="s">
         <v>603</v>
       </c>
-      <c r="D135" s="28" t="s">
+      <c r="D135" s="27" t="s">
         <v>607</v>
       </c>
       <c r="E135" s="1" t="s">
@@ -6978,7 +6982,7 @@
       <c r="C136" s="1" t="s">
         <v>604</v>
       </c>
-      <c r="D136" s="28" t="s">
+      <c r="D136" s="27" t="s">
         <v>608</v>
       </c>
       <c r="E136" s="1" t="s">
@@ -6998,7 +7002,7 @@
       <c r="C137" s="1" t="s">
         <v>609</v>
       </c>
-      <c r="D137" s="27" t="s">
+      <c r="D137" s="26" t="s">
         <v>620</v>
       </c>
       <c r="E137" s="1" t="s">
@@ -7076,7 +7080,7 @@
       </c>
       <c r="E141" s="1">
         <f>SUBTOTAL(103,Table1[Variable type])</f>
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="F141" s="1">
         <f>SUBTOTAL(103,Table1[Data source / Friendly Name])</f>
@@ -7115,6 +7119,22 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
       <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup displayEmptyCellsAs="gap" markers="1" high="1" low="1" xr2:uid="{8EE07F88-13A6-4284-BDAE-703BC4E55F90}">
+          <x14:colorSeries rgb="FF0070C0"/>
+          <x14:colorNegative rgb="FF000000"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers rgb="FF000000"/>
+          <x14:colorFirst rgb="FF000000"/>
+          <x14:colorLast rgb="FF000000"/>
+          <x14:colorHigh rgb="FF000000"/>
+          <x14:colorLow rgb="FF000000"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Draft- Data Dictionary'!C141:I141</xm:f>
+              <xm:sqref>J141</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
         <x14:sparklineGroup type="column" displayEmptyCellsAs="gap" xr2:uid="{9678263F-BAEB-48A3-82AC-EA2CB30D2801}">
           <x14:colorSeries rgb="FF376092"/>
           <x14:colorNegative rgb="FFD00000"/>
@@ -7128,22 +7148,6 @@
             <x14:sparkline>
               <xm:f>'Draft- Data Dictionary'!C141:I141</xm:f>
               <xm:sqref>K141</xm:sqref>
-            </x14:sparkline>
-          </x14:sparklines>
-        </x14:sparklineGroup>
-        <x14:sparklineGroup displayEmptyCellsAs="gap" markers="1" high="1" low="1" xr2:uid="{8EE07F88-13A6-4284-BDAE-703BC4E55F90}">
-          <x14:colorSeries rgb="FF0070C0"/>
-          <x14:colorNegative rgb="FF000000"/>
-          <x14:colorAxis rgb="FF000000"/>
-          <x14:colorMarkers rgb="FF000000"/>
-          <x14:colorFirst rgb="FF000000"/>
-          <x14:colorLast rgb="FF000000"/>
-          <x14:colorHigh rgb="FF000000"/>
-          <x14:colorLow rgb="FF000000"/>
-          <x14:sparklines>
-            <x14:sparkline>
-              <xm:f>'Draft- Data Dictionary'!C141:I141</xm:f>
-              <xm:sqref>J141</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -7168,10 +7172,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="28" t="s">
         <v>454</v>
       </c>
-      <c r="C1" s="25"/>
+      <c r="C1" s="28"/>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" t="s">

</xml_diff>